<commit_message>
File upload box added
</commit_message>
<xml_diff>
--- a/uploads/children_names.xlsx
+++ b/uploads/children_names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python_stuff\Family_Sort_Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96CF6F57-0C0B-4643-B114-3105D280A3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE68FD41-5085-4F64-AE22-828791E97A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4980" yWindow="1680" windowWidth="29040" windowHeight="15840" xr2:uid="{0D17AE3C-D650-4A1A-ABD5-581312FC75DE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Emma</t>
   </si>
@@ -144,63 +144,6 @@
   </si>
   <si>
     <t>Owen</t>
-  </si>
-  <si>
-    <t>Victoria</t>
-  </si>
-  <si>
-    <t>Gabriel</t>
-  </si>
-  <si>
-    <t>Luna</t>
-  </si>
-  <si>
-    <t>Matthew</t>
-  </si>
-  <si>
-    <t>Grace</t>
-  </si>
-  <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>Chloe</t>
-  </si>
-  <si>
-    <t>Joseph</t>
-  </si>
-  <si>
-    <t>Penelope</t>
-  </si>
-  <si>
-    <t>Samuel</t>
-  </si>
-  <si>
-    <t>Layla</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Riley</t>
-  </si>
-  <si>
-    <t>Luke</t>
-  </si>
-  <si>
-    <t>Zoey</t>
-  </si>
-  <si>
-    <t>Andrew</t>
-  </si>
-  <si>
-    <t>Nora</t>
-  </si>
-  <si>
-    <t>Nathan</t>
-  </si>
-  <si>
-    <t>Lily</t>
   </si>
 </sst>
 </file>
@@ -572,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF92E861-71EF-4AE8-A443-BE3EBC7A7CAA}">
-  <dimension ref="A1:A55"/>
+  <dimension ref="A1:A36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A55"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,101 +703,6 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>54</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>